<commit_message>
logging times more accurately
in a separate version
</commit_message>
<xml_diff>
--- a/domDecom/scalingAndComparisons.xlsx
+++ b/domDecom/scalingAndComparisons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djc23551\Fortran\3DSpace\domDecom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FD86F6-7A59-44FB-AAAC-E0A8E048F280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754D633A-91AB-46D9-82DD-0137F120431B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{B9CF305C-A12F-4BBA-AE2C-DC494FEA2EEA}"/>
+    <workbookView xWindow="-38510" yWindow="-7330" windowWidth="38620" windowHeight="21220" xr2:uid="{B9CF305C-A12F-4BBA-AE2C-DC494FEA2EEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Domain Decomp" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="69">
   <si>
     <t xml:space="preserve"> 1,   1,   1</t>
   </si>
@@ -220,6 +220,30 @@
   </si>
   <si>
     <t>Domain Decomposition: 0.05 Cutoff, 50000 more particles per process added, Omitted nprocs that change Cutoff, O3 optimisation</t>
+  </si>
+  <si>
+    <t>Nparts</t>
+  </si>
+  <si>
+    <t>Note: For this, it is only timing from the first instance of particle counting to the final addition</t>
+  </si>
+  <si>
+    <t>Domain Decomposition: 0.05 Cutoff, 50000 more particles per process added, Omitted nprocs that change Cutoff, O3 optimisation, Space grows as particles increase, Rand Seed 4, Original 50:(1,1,1)</t>
+  </si>
+  <si>
+    <t>Domain Decomposition: 1 Million particles, 0.05 Cutoff, O3, Overall Time - Changed Cutoff Omitted</t>
+  </si>
+  <si>
+    <t>4,   4,   2</t>
+  </si>
+  <si>
+    <t>6,   2,   3</t>
+  </si>
+  <si>
+    <t>4,   6,   2</t>
+  </si>
+  <si>
+    <t>4,   4,   4</t>
   </si>
 </sst>
 </file>
@@ -467,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -543,6 +567,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2573,7 +2604,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.6600596553879072E-2"/>
+          <c:y val="9.6036614112349164E-2"/>
+          <c:w val="0.95415246706124501"/>
+          <c:h val="0.83978392427082504"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -3801,6 +3842,460 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Strong Scaling</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Domain Decomp'!$C$161:$C$184</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Domain Decomp'!$R$161:$R$184</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1676206999059451</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8712482557402002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.8424076317383395</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.497224731350258</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.490278040476642</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.649010156653471</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31.076333907056799</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35.062714424425515</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.614801023970209</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46.797408114042987</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56.47444285155742</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>66.20754774637129</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>72.608646112600525</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80.784563758389268</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70.979262899262906</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>67.873711690074671</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>78.477826743133122</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>84.119658340882623</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>93.84819520646839</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>104.97296511627907</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>119.31943093162002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>140.52374878391524</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>171.06869144120432</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5917-4EB7-B66E-3D3FB24D62F2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="443753824"/>
+        <c:axId val="443761984"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="443753824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="443761984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="443761984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="443753824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="10"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4041,6 +4536,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -6622,6 +7157,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7475,6 +8526,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>53975</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84F88C92-7867-7919-6E1F-0452C6A0FD63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7880,10 +8967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6BFA83E-ABBE-4898-9E21-4EF30DE0B370}">
-  <dimension ref="A1:AQ104"/>
+  <dimension ref="A1:AQ184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S96" sqref="S96"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q196" activeCellId="1" sqref="H184 Q196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12587,7 +13674,7 @@
         <v>6.35</v>
       </c>
       <c r="AF87" s="4">
-        <f t="shared" ref="AF85:AF103" si="14">AVERAGE(W87:AE87)</f>
+        <f t="shared" ref="AF87:AF92" si="14">AVERAGE(W87:AE87)</f>
         <v>4.9842222222222228</v>
       </c>
       <c r="AG87" s="4"/>
@@ -12972,7 +14059,7 @@
         <v>10.451000000000001</v>
       </c>
       <c r="AF94" s="4">
-        <f t="shared" ref="AF94:AF104" si="15">AVERAGE(W94:AE94)</f>
+        <f t="shared" ref="AF94" si="15">AVERAGE(W94:AE94)</f>
         <v>10.658777777777779</v>
       </c>
       <c r="AG94" s="4"/>
@@ -13082,7 +14169,7 @@
         <v>15.148999999999999</v>
       </c>
       <c r="AF96" s="4">
-        <f t="shared" ref="AF96:AF104" si="16">AVERAGE(W96:AE96)</f>
+        <f t="shared" ref="AF96:AF103" si="16">AVERAGE(W96:AE96)</f>
         <v>13.8</v>
       </c>
       <c r="AG96" s="4"/>
@@ -13539,8 +14626,1668 @@
         <v>9.6907420285148482E-2</v>
       </c>
     </row>
+    <row r="130" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="131" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B131" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C131" s="30"/>
+      <c r="D131" s="30"/>
+      <c r="E131" s="30"/>
+      <c r="F131" s="30"/>
+      <c r="G131" s="30"/>
+      <c r="H131" s="30"/>
+      <c r="I131" s="30"/>
+      <c r="J131" s="31"/>
+    </row>
+    <row r="132" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B132" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C132" s="30"/>
+      <c r="D132" s="30"/>
+      <c r="E132" s="30"/>
+      <c r="F132" s="30"/>
+      <c r="G132" s="30"/>
+      <c r="H132" s="30"/>
+      <c r="I132" s="30"/>
+      <c r="J132" s="30"/>
+      <c r="K132" s="30"/>
+      <c r="L132" s="30"/>
+      <c r="M132" s="30"/>
+      <c r="N132" s="30"/>
+      <c r="O132" s="30"/>
+      <c r="P132" s="30"/>
+      <c r="Q132" s="30"/>
+      <c r="R132" s="31"/>
+      <c r="S132" s="41"/>
+      <c r="T132" s="42"/>
+    </row>
+    <row r="133" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B133" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D133" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E133" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F133" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G133" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H133" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="I133" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J133" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K133" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="L133" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="M133" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="N133" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="O133" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q133" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R133" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="S133" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="134" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B134" s="3">
+        <v>50000</v>
+      </c>
+      <c r="C134" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D134" s="3">
+        <v>1</v>
+      </c>
+      <c r="E134" s="6">
+        <v>2.9</v>
+      </c>
+      <c r="F134">
+        <v>3.0009999999999999</v>
+      </c>
+      <c r="G134" s="7">
+        <v>2.9169999999999998</v>
+      </c>
+      <c r="H134" s="7">
+        <v>3.1970000000000001</v>
+      </c>
+      <c r="I134" s="7">
+        <v>2.899</v>
+      </c>
+      <c r="J134" s="7">
+        <v>2.9689999999999999</v>
+      </c>
+      <c r="K134" s="7">
+        <v>2.956</v>
+      </c>
+      <c r="L134" s="7"/>
+      <c r="M134" s="7"/>
+      <c r="N134" s="22"/>
+      <c r="O134" s="3">
+        <f>AVERAGE(F134:N134)</f>
+        <v>2.9898333333333333</v>
+      </c>
+      <c r="P134" s="3"/>
+      <c r="Q134" s="3">
+        <f>MAX(E134:G134)</f>
+        <v>3.0009999999999999</v>
+      </c>
+      <c r="R134" s="3">
+        <f>MIN(E134:G134)</f>
+        <v>2.9</v>
+      </c>
+      <c r="S134" s="3">
+        <f>O134/O134</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B135" s="4">
+        <v>100000</v>
+      </c>
+      <c r="C135" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D135" s="4">
+        <v>2</v>
+      </c>
+      <c r="E135" s="10">
+        <v>3.2719999999999998</v>
+      </c>
+      <c r="F135">
+        <v>3.0920000000000001</v>
+      </c>
+      <c r="G135">
+        <v>3.2109999999999999</v>
+      </c>
+      <c r="H135">
+        <v>3.68</v>
+      </c>
+      <c r="I135">
+        <v>3.202</v>
+      </c>
+      <c r="N135" s="13"/>
+      <c r="O135" s="4">
+        <f>AVERAGE(F135:N135)</f>
+        <v>3.2962500000000001</v>
+      </c>
+      <c r="P135" s="4"/>
+      <c r="Q135" s="4">
+        <f t="shared" ref="Q135:Q153" si="17">MAX(E135:G135)</f>
+        <v>3.2719999999999998</v>
+      </c>
+      <c r="R135" s="4">
+        <f t="shared" ref="R135:R153" si="18">MIN(E135:G135)</f>
+        <v>3.0920000000000001</v>
+      </c>
+      <c r="S135" s="4">
+        <f>O134/O135</f>
+        <v>0.90704082922512952</v>
+      </c>
+    </row>
+    <row r="136" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B136" s="4">
+        <v>150000</v>
+      </c>
+      <c r="C136" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D136" s="4">
+        <v>3</v>
+      </c>
+      <c r="E136" s="10">
+        <v>2.968</v>
+      </c>
+      <c r="F136">
+        <v>3.2029999999999998</v>
+      </c>
+      <c r="G136">
+        <v>3.2290000000000001</v>
+      </c>
+      <c r="H136">
+        <v>3.206</v>
+      </c>
+      <c r="I136">
+        <v>3.052</v>
+      </c>
+      <c r="J136">
+        <v>2.9830000000000001</v>
+      </c>
+      <c r="N136" s="13"/>
+      <c r="O136" s="4">
+        <f t="shared" ref="O136:O141" si="19">AVERAGE(F136:N136)</f>
+        <v>3.1345999999999998</v>
+      </c>
+      <c r="P136" s="4"/>
+      <c r="Q136" s="4">
+        <f t="shared" si="17"/>
+        <v>3.2290000000000001</v>
+      </c>
+      <c r="R136" s="4">
+        <f t="shared" si="18"/>
+        <v>2.968</v>
+      </c>
+      <c r="S136" s="4">
+        <f>O134/O136</f>
+        <v>0.95381654224887813</v>
+      </c>
+    </row>
+    <row r="137" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B137" s="4">
+        <v>200000</v>
+      </c>
+      <c r="C137" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D137" s="4">
+        <v>4</v>
+      </c>
+      <c r="E137" s="10">
+        <v>3.9689999999999999</v>
+      </c>
+      <c r="F137">
+        <v>3.3959999999999999</v>
+      </c>
+      <c r="G137">
+        <v>3.4750000000000001</v>
+      </c>
+      <c r="H137">
+        <v>3.2330000000000001</v>
+      </c>
+      <c r="I137">
+        <v>2.8260000000000001</v>
+      </c>
+      <c r="J137">
+        <v>3.9220000000000002</v>
+      </c>
+      <c r="N137" s="13"/>
+      <c r="O137" s="4">
+        <f t="shared" si="19"/>
+        <v>3.3704000000000001</v>
+      </c>
+      <c r="P137" s="4"/>
+      <c r="Q137" s="4">
+        <f t="shared" si="17"/>
+        <v>3.9689999999999999</v>
+      </c>
+      <c r="R137" s="4">
+        <f t="shared" si="18"/>
+        <v>3.3959999999999999</v>
+      </c>
+      <c r="S137" s="4">
+        <f>O134/O137</f>
+        <v>0.88708560803861058</v>
+      </c>
+    </row>
+    <row r="138" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B138" s="4">
+        <v>250000</v>
+      </c>
+      <c r="C138" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D138" s="4">
+        <v>5</v>
+      </c>
+      <c r="E138" s="10">
+        <v>3.645</v>
+      </c>
+      <c r="F138">
+        <v>4.0940000000000003</v>
+      </c>
+      <c r="G138">
+        <v>3.867</v>
+      </c>
+      <c r="H138">
+        <v>3.7919999999999998</v>
+      </c>
+      <c r="I138">
+        <v>3.9889999999999999</v>
+      </c>
+      <c r="J138">
+        <v>3.6829999999999998</v>
+      </c>
+      <c r="N138" s="13"/>
+      <c r="O138" s="4">
+        <f t="shared" si="19"/>
+        <v>3.8850000000000002</v>
+      </c>
+      <c r="P138" s="4"/>
+      <c r="Q138" s="4">
+        <f t="shared" si="17"/>
+        <v>4.0940000000000003</v>
+      </c>
+      <c r="R138" s="4">
+        <f t="shared" si="18"/>
+        <v>3.645</v>
+      </c>
+      <c r="S138" s="4">
+        <f>O134/O138</f>
+        <v>0.7695838695838696</v>
+      </c>
+    </row>
+    <row r="139" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B139" s="4">
+        <v>300000</v>
+      </c>
+      <c r="C139" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D139" s="4">
+        <v>6</v>
+      </c>
+      <c r="E139" s="10">
+        <v>3.89</v>
+      </c>
+      <c r="F139">
+        <v>4.5750000000000002</v>
+      </c>
+      <c r="G139">
+        <v>4.9980000000000002</v>
+      </c>
+      <c r="H139">
+        <v>4.5019999999999998</v>
+      </c>
+      <c r="I139">
+        <v>5.0410000000000004</v>
+      </c>
+      <c r="N139" s="13"/>
+      <c r="O139" s="4">
+        <f t="shared" si="19"/>
+        <v>4.7789999999999999</v>
+      </c>
+      <c r="P139" s="4"/>
+      <c r="Q139" s="4">
+        <f t="shared" si="17"/>
+        <v>4.9980000000000002</v>
+      </c>
+      <c r="R139" s="4">
+        <f t="shared" si="18"/>
+        <v>3.89</v>
+      </c>
+      <c r="S139" s="4">
+        <f>O134/O139</f>
+        <v>0.62561902769059075</v>
+      </c>
+    </row>
+    <row r="140" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B140" s="4">
+        <v>350000</v>
+      </c>
+      <c r="C140" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D140" s="4">
+        <v>7</v>
+      </c>
+      <c r="E140" s="10">
+        <v>4.9420000000000002</v>
+      </c>
+      <c r="F140">
+        <v>4.234</v>
+      </c>
+      <c r="G140">
+        <v>4.7789999999999999</v>
+      </c>
+      <c r="H140">
+        <v>4.4050000000000002</v>
+      </c>
+      <c r="I140">
+        <v>4.8769999999999998</v>
+      </c>
+      <c r="N140" s="13"/>
+      <c r="O140" s="4">
+        <f t="shared" si="19"/>
+        <v>4.5737499999999995</v>
+      </c>
+      <c r="P140" s="4"/>
+      <c r="Q140" s="4">
+        <f t="shared" si="17"/>
+        <v>4.9420000000000002</v>
+      </c>
+      <c r="R140" s="4">
+        <f t="shared" si="18"/>
+        <v>4.234</v>
+      </c>
+      <c r="S140" s="4">
+        <f>O134/O140</f>
+        <v>0.65369408763778813</v>
+      </c>
+    </row>
+    <row r="141" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B141" s="4">
+        <v>400000</v>
+      </c>
+      <c r="C141" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D141" s="4">
+        <v>8</v>
+      </c>
+      <c r="E141" s="10"/>
+      <c r="N141" s="13"/>
+      <c r="O141" s="4" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P141" s="4"/>
+      <c r="Q141" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R141" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S141" s="4" t="e">
+        <f>O134/O141</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="142" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B142" s="4">
+        <v>450000</v>
+      </c>
+      <c r="C142" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142" s="4">
+        <v>9</v>
+      </c>
+      <c r="E142" s="10"/>
+      <c r="N142" s="13"/>
+      <c r="O142" s="4" t="e">
+        <f>AVERAGE(F142:N142)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P142" s="4"/>
+      <c r="Q142" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R142" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S142" s="4" t="e">
+        <f>O134/O142</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="143" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B143" s="4">
+        <v>500000</v>
+      </c>
+      <c r="C143" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D143" s="4">
+        <v>10</v>
+      </c>
+      <c r="E143" s="10"/>
+      <c r="O143" s="4" t="e">
+        <f t="shared" ref="O143" si="20">AVERAGE(F143:N143)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P143" s="4"/>
+      <c r="Q143" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R143" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S143" s="4" t="e">
+        <f>O134/O143</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="144" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B144" s="4">
+        <v>550000</v>
+      </c>
+      <c r="C144" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D144" s="4">
+        <v>12</v>
+      </c>
+      <c r="E144" s="10"/>
+      <c r="N144" s="13"/>
+      <c r="O144" s="4" t="e">
+        <f>AVERAGE(F144:N144)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P144" s="4"/>
+      <c r="Q144" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R144" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S144" s="4" t="e">
+        <f>O134/O144</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="145" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B145" s="4">
+        <v>600000</v>
+      </c>
+      <c r="C145" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D145" s="4">
+        <v>14</v>
+      </c>
+      <c r="E145" s="10"/>
+      <c r="N145" s="13"/>
+      <c r="O145" s="4" t="e">
+        <f t="shared" ref="O145:O152" si="21">AVERAGE(F145:N145)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P145" s="4"/>
+      <c r="Q145" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R145" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S145" s="4" t="e">
+        <f>O134/O145</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="146" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B146" s="4">
+        <v>650000</v>
+      </c>
+      <c r="C146" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146" s="4">
+        <v>15</v>
+      </c>
+      <c r="E146" s="10"/>
+      <c r="N146" s="13"/>
+      <c r="O146" s="4" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P146" s="4"/>
+      <c r="Q146" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R146" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S146" s="4" t="e">
+        <f>O134/O146</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="147" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B147" s="4">
+        <v>700000</v>
+      </c>
+      <c r="C147" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D147" s="4">
+        <v>16</v>
+      </c>
+      <c r="E147" s="10"/>
+      <c r="N147" s="13"/>
+      <c r="O147" s="4" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P147" s="4"/>
+      <c r="Q147" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R147" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S147" s="4" t="e">
+        <f>O134/O147</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="148" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B148" s="4">
+        <v>750000</v>
+      </c>
+      <c r="C148" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D148" s="4">
+        <v>18</v>
+      </c>
+      <c r="E148" s="10"/>
+      <c r="N148" s="13"/>
+      <c r="O148" s="4" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P148" s="4"/>
+      <c r="Q148" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R148" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S148" s="4" t="e">
+        <f>O134/O148</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="149" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B149" s="4">
+        <v>800000</v>
+      </c>
+      <c r="C149" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D149" s="4">
+        <v>20</v>
+      </c>
+      <c r="E149" s="10"/>
+      <c r="N149" s="13"/>
+      <c r="O149" s="4" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P149" s="4"/>
+      <c r="Q149" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R149" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S149" s="4" t="e">
+        <f>O134/O149</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="150" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B150" s="4">
+        <v>850000</v>
+      </c>
+      <c r="C150" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D150" s="4">
+        <v>21</v>
+      </c>
+      <c r="E150" s="10"/>
+      <c r="N150" s="13"/>
+      <c r="O150" s="4" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P150" s="4"/>
+      <c r="Q150" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R150" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S150" s="4" t="e">
+        <f>O134/O150</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="151" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B151" s="4">
+        <v>900000</v>
+      </c>
+      <c r="C151" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D151" s="4">
+        <v>24</v>
+      </c>
+      <c r="E151" s="10"/>
+      <c r="N151" s="13"/>
+      <c r="O151" s="4" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P151" s="4"/>
+      <c r="Q151" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R151" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S151" s="4" t="e">
+        <f>O134/O151</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="152" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B152" s="4">
+        <v>950000</v>
+      </c>
+      <c r="C152" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D152" s="4">
+        <v>25</v>
+      </c>
+      <c r="E152" s="10"/>
+      <c r="N152" s="13"/>
+      <c r="O152" s="4" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P152" s="4"/>
+      <c r="Q152" s="4">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R152" s="4">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S152" s="4" t="e">
+        <f>O134/O152</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="153" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B153" s="5">
+        <v>1000000</v>
+      </c>
+      <c r="C153" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D153" s="5">
+        <v>27</v>
+      </c>
+      <c r="E153" s="14"/>
+      <c r="F153" s="15"/>
+      <c r="G153" s="15"/>
+      <c r="H153" s="15"/>
+      <c r="I153" s="15"/>
+      <c r="J153" s="15"/>
+      <c r="K153" s="15"/>
+      <c r="L153" s="15"/>
+      <c r="M153" s="15"/>
+      <c r="N153" s="16"/>
+      <c r="O153" s="5" t="e">
+        <f>AVERAGE(F153:N153)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P153" s="5"/>
+      <c r="Q153" s="5">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R153" s="5">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="S153" s="5" t="e">
+        <f>O134/O153</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="158" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="159" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B159" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C159" s="30"/>
+      <c r="D159" s="30"/>
+      <c r="E159" s="30"/>
+      <c r="F159" s="30"/>
+      <c r="G159" s="30"/>
+      <c r="H159" s="30"/>
+      <c r="I159" s="30"/>
+      <c r="J159" s="30"/>
+      <c r="K159" s="30"/>
+      <c r="L159" s="30"/>
+      <c r="M159" s="30"/>
+      <c r="N159" s="30"/>
+      <c r="O159" s="30"/>
+      <c r="P159" s="30"/>
+      <c r="Q159" s="30"/>
+      <c r="R159" s="1"/>
+    </row>
+    <row r="160" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B160" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C160" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D160" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E160" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F160" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G160" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H160" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="I160" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J160" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="K160" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="L160" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="M160" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="N160" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="O160" s="40"/>
+      <c r="P160" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q160" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="R160" s="17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="161" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B161" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C161" s="3">
+        <v>1</v>
+      </c>
+      <c r="D161">
+        <v>649.99260000000004</v>
+      </c>
+      <c r="E161">
+        <v>649.99260000000004</v>
+      </c>
+      <c r="G161" s="11"/>
+      <c r="H161" s="11"/>
+      <c r="I161" s="11"/>
+      <c r="J161" s="11"/>
+      <c r="K161" s="11"/>
+      <c r="L161" s="11"/>
+      <c r="M161" s="11"/>
+      <c r="N161" s="27">
+        <f>AVERAGE(D161:M161)</f>
+        <v>649.99260000000004</v>
+      </c>
+      <c r="O161" s="28"/>
+      <c r="P161" s="4">
+        <f>MAX(D161:F161)</f>
+        <v>649.99260000000004</v>
+      </c>
+      <c r="Q161" s="4">
+        <f>MIN(D161:F161)</f>
+        <v>649.99260000000004</v>
+      </c>
+      <c r="R161" s="13">
+        <f>N161/N161</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B162" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C162" s="4">
+        <v>2</v>
+      </c>
+      <c r="D162">
+        <v>205.19900000000001</v>
+      </c>
+      <c r="E162">
+        <v>205.19900000000001</v>
+      </c>
+      <c r="I162" s="11"/>
+      <c r="J162" s="11"/>
+      <c r="K162" s="11"/>
+      <c r="L162" s="11"/>
+      <c r="M162" s="11"/>
+      <c r="N162" s="27">
+        <f t="shared" ref="N162:N184" si="22">AVERAGE(D162:M162)</f>
+        <v>205.19900000000001</v>
+      </c>
+      <c r="O162" s="28"/>
+      <c r="P162" s="4">
+        <f t="shared" ref="P162:P180" si="23">MAX(D162:F162)</f>
+        <v>205.19900000000001</v>
+      </c>
+      <c r="Q162" s="4">
+        <f t="shared" ref="Q162:Q180" si="24">MIN(D162:F162)</f>
+        <v>205.19900000000001</v>
+      </c>
+      <c r="R162" s="13">
+        <f>N161/N162</f>
+        <v>3.1676206999059451</v>
+      </c>
+    </row>
+    <row r="163" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B163" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C163" s="4">
+        <v>3</v>
+      </c>
+      <c r="D163">
+        <v>94.596000000000004</v>
+      </c>
+      <c r="E163">
+        <v>94.596000000000004</v>
+      </c>
+      <c r="I163" s="11"/>
+      <c r="J163" s="11"/>
+      <c r="K163" s="11"/>
+      <c r="L163" s="11"/>
+      <c r="M163" s="11"/>
+      <c r="N163" s="27">
+        <f t="shared" si="22"/>
+        <v>94.596000000000004</v>
+      </c>
+      <c r="O163" s="28"/>
+      <c r="P163" s="4">
+        <f t="shared" si="23"/>
+        <v>94.596000000000004</v>
+      </c>
+      <c r="Q163" s="4">
+        <f t="shared" si="24"/>
+        <v>94.596000000000004</v>
+      </c>
+      <c r="R163" s="13">
+        <f>N161/N163</f>
+        <v>6.8712482557402002</v>
+      </c>
+    </row>
+    <row r="164" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B164" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C164" s="4">
+        <v>4</v>
+      </c>
+      <c r="D164">
+        <v>66.040000000000006</v>
+      </c>
+      <c r="E164">
+        <v>66.040000000000006</v>
+      </c>
+      <c r="N164" s="27">
+        <f t="shared" si="22"/>
+        <v>66.040000000000006</v>
+      </c>
+      <c r="O164" s="28"/>
+      <c r="P164" s="4">
+        <f t="shared" si="23"/>
+        <v>66.040000000000006</v>
+      </c>
+      <c r="Q164" s="4">
+        <f t="shared" si="24"/>
+        <v>66.040000000000006</v>
+      </c>
+      <c r="R164" s="13">
+        <f>N161/N164</f>
+        <v>9.8424076317383395</v>
+      </c>
+    </row>
+    <row r="165" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B165" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C165" s="4">
+        <v>5</v>
+      </c>
+      <c r="D165">
+        <v>40.729999999999997</v>
+      </c>
+      <c r="E165">
+        <v>55.585000000000001</v>
+      </c>
+      <c r="N165" s="27">
+        <f t="shared" si="22"/>
+        <v>48.157499999999999</v>
+      </c>
+      <c r="O165" s="28"/>
+      <c r="P165" s="4">
+        <f t="shared" si="23"/>
+        <v>55.585000000000001</v>
+      </c>
+      <c r="Q165" s="4">
+        <f t="shared" si="24"/>
+        <v>40.729999999999997</v>
+      </c>
+      <c r="R165" s="13">
+        <f>N161/N165</f>
+        <v>13.497224731350258</v>
+      </c>
+    </row>
+    <row r="166" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B166" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C166" s="4">
+        <v>6</v>
+      </c>
+      <c r="D166">
+        <v>28.544</v>
+      </c>
+      <c r="E166">
+        <v>34.9</v>
+      </c>
+      <c r="N166" s="27">
+        <f t="shared" si="22"/>
+        <v>31.722000000000001</v>
+      </c>
+      <c r="O166" s="28"/>
+      <c r="P166" s="4">
+        <f t="shared" si="23"/>
+        <v>34.9</v>
+      </c>
+      <c r="Q166" s="4">
+        <f t="shared" si="24"/>
+        <v>28.544</v>
+      </c>
+      <c r="R166" s="13">
+        <f>N161/N166</f>
+        <v>20.490278040476642</v>
+      </c>
+    </row>
+    <row r="167" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B167" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C167" s="4">
+        <v>7</v>
+      </c>
+      <c r="D167">
+        <v>33.314</v>
+      </c>
+      <c r="E167">
+        <v>36.393999999999998</v>
+      </c>
+      <c r="N167" s="27">
+        <f t="shared" si="22"/>
+        <v>34.853999999999999</v>
+      </c>
+      <c r="O167" s="28"/>
+      <c r="P167" s="4">
+        <f t="shared" si="23"/>
+        <v>36.393999999999998</v>
+      </c>
+      <c r="Q167" s="4">
+        <f t="shared" si="24"/>
+        <v>33.314</v>
+      </c>
+      <c r="R167" s="13">
+        <f>N161/N167</f>
+        <v>18.649010156653471</v>
+      </c>
+    </row>
+    <row r="168" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B168" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C168" s="4">
+        <v>8</v>
+      </c>
+      <c r="D168">
+        <v>20.231000000000002</v>
+      </c>
+      <c r="E168">
+        <v>21.600999999999999</v>
+      </c>
+      <c r="N168" s="27">
+        <f t="shared" si="22"/>
+        <v>20.916</v>
+      </c>
+      <c r="O168" s="28"/>
+      <c r="P168" s="4">
+        <f>MAX(D168:F168)</f>
+        <v>21.600999999999999</v>
+      </c>
+      <c r="Q168" s="4">
+        <f>MIN(D168:F168)</f>
+        <v>20.231000000000002</v>
+      </c>
+      <c r="R168" s="13">
+        <f>N161/N168</f>
+        <v>31.076333907056799</v>
+      </c>
+    </row>
+    <row r="169" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B169" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C169" s="4">
+        <v>9</v>
+      </c>
+      <c r="D169">
+        <v>18.986999999999998</v>
+      </c>
+      <c r="E169">
+        <v>18.088999999999999</v>
+      </c>
+      <c r="N169" s="27">
+        <f t="shared" si="22"/>
+        <v>18.537999999999997</v>
+      </c>
+      <c r="O169" s="28"/>
+      <c r="P169" s="4">
+        <f t="shared" si="23"/>
+        <v>18.986999999999998</v>
+      </c>
+      <c r="Q169" s="4">
+        <f t="shared" si="24"/>
+        <v>18.088999999999999</v>
+      </c>
+      <c r="R169" s="13">
+        <f>N161/N169</f>
+        <v>35.062714424425515</v>
+      </c>
+    </row>
+    <row r="170" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B170" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C170" s="4">
+        <v>10</v>
+      </c>
+      <c r="D170">
+        <v>20.183</v>
+      </c>
+      <c r="E170">
+        <v>18.489999999999998</v>
+      </c>
+      <c r="N170" s="27">
+        <f t="shared" si="22"/>
+        <v>19.336500000000001</v>
+      </c>
+      <c r="O170" s="28"/>
+      <c r="P170" s="4">
+        <f t="shared" si="23"/>
+        <v>20.183</v>
+      </c>
+      <c r="Q170" s="4">
+        <f t="shared" si="24"/>
+        <v>18.489999999999998</v>
+      </c>
+      <c r="R170" s="13">
+        <f>N161/N170</f>
+        <v>33.614801023970209</v>
+      </c>
+    </row>
+    <row r="171" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B171" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C171" s="4">
+        <v>12</v>
+      </c>
+      <c r="D171">
+        <v>12.340999999999999</v>
+      </c>
+      <c r="E171">
+        <v>15.438000000000001</v>
+      </c>
+      <c r="N171" s="27">
+        <f t="shared" si="22"/>
+        <v>13.8895</v>
+      </c>
+      <c r="O171" s="28"/>
+      <c r="P171" s="4">
+        <f t="shared" si="23"/>
+        <v>15.438000000000001</v>
+      </c>
+      <c r="Q171" s="4">
+        <f t="shared" si="24"/>
+        <v>12.340999999999999</v>
+      </c>
+      <c r="R171" s="13">
+        <f>N161/N171</f>
+        <v>46.797408114042987</v>
+      </c>
+    </row>
+    <row r="172" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B172" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C172" s="4">
+        <v>14</v>
+      </c>
+      <c r="D172">
+        <v>10.989000000000001</v>
+      </c>
+      <c r="E172">
+        <v>12.03</v>
+      </c>
+      <c r="N172" s="27">
+        <f t="shared" si="22"/>
+        <v>11.509499999999999</v>
+      </c>
+      <c r="O172" s="28"/>
+      <c r="P172" s="4">
+        <f t="shared" si="23"/>
+        <v>12.03</v>
+      </c>
+      <c r="Q172" s="4">
+        <f t="shared" si="24"/>
+        <v>10.989000000000001</v>
+      </c>
+      <c r="R172" s="13">
+        <f>N161/N172</f>
+        <v>56.47444285155742</v>
+      </c>
+    </row>
+    <row r="173" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B173" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C173" s="4">
+        <v>15</v>
+      </c>
+      <c r="D173">
+        <v>9.9</v>
+      </c>
+      <c r="E173">
+        <v>9.7349999999999994</v>
+      </c>
+      <c r="N173" s="27">
+        <f t="shared" si="22"/>
+        <v>9.817499999999999</v>
+      </c>
+      <c r="O173" s="28"/>
+      <c r="P173" s="4">
+        <f t="shared" si="23"/>
+        <v>9.9</v>
+      </c>
+      <c r="Q173" s="4">
+        <f t="shared" si="24"/>
+        <v>9.7349999999999994</v>
+      </c>
+      <c r="R173" s="13">
+        <f>N161/N173</f>
+        <v>66.20754774637129</v>
+      </c>
+    </row>
+    <row r="174" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B174" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C174" s="4">
+        <v>16</v>
+      </c>
+      <c r="D174">
+        <v>8.8350000000000009</v>
+      </c>
+      <c r="E174">
+        <v>9.0690000000000008</v>
+      </c>
+      <c r="N174" s="27">
+        <f t="shared" si="22"/>
+        <v>8.9520000000000017</v>
+      </c>
+      <c r="O174" s="28"/>
+      <c r="P174" s="4">
+        <f>MAX(D174:F174)</f>
+        <v>9.0690000000000008</v>
+      </c>
+      <c r="Q174" s="4">
+        <f>MIN(D174:F174)</f>
+        <v>8.8350000000000009</v>
+      </c>
+      <c r="R174" s="13">
+        <f>N161/N174</f>
+        <v>72.608646112600525</v>
+      </c>
+    </row>
+    <row r="175" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B175" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C175" s="4">
+        <v>18</v>
+      </c>
+      <c r="D175">
+        <v>7.9450000000000003</v>
+      </c>
+      <c r="E175">
+        <v>8.1470000000000002</v>
+      </c>
+      <c r="N175" s="27">
+        <f t="shared" si="22"/>
+        <v>8.0459999999999994</v>
+      </c>
+      <c r="O175" s="28"/>
+      <c r="P175" s="4">
+        <f t="shared" si="23"/>
+        <v>8.1470000000000002</v>
+      </c>
+      <c r="Q175" s="4">
+        <f t="shared" si="24"/>
+        <v>7.9450000000000003</v>
+      </c>
+      <c r="R175" s="13">
+        <f>N161/N175</f>
+        <v>80.784563758389268</v>
+      </c>
+    </row>
+    <row r="176" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B176" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C176" s="4">
+        <v>20</v>
+      </c>
+      <c r="D176">
+        <v>9.0640000000000001</v>
+      </c>
+      <c r="E176">
+        <v>9.2509999999999994</v>
+      </c>
+      <c r="N176" s="27">
+        <f t="shared" si="22"/>
+        <v>9.1574999999999989</v>
+      </c>
+      <c r="O176" s="28"/>
+      <c r="P176" s="4">
+        <f t="shared" si="23"/>
+        <v>9.2509999999999994</v>
+      </c>
+      <c r="Q176" s="4">
+        <f t="shared" si="24"/>
+        <v>9.0640000000000001</v>
+      </c>
+      <c r="R176" s="13">
+        <f>N161/N176</f>
+        <v>70.979262899262906</v>
+      </c>
+    </row>
+    <row r="177" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B177" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C177" s="4">
+        <v>21</v>
+      </c>
+      <c r="D177">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="E177">
+        <v>9.3629999999999995</v>
+      </c>
+      <c r="N177" s="27">
+        <f t="shared" si="22"/>
+        <v>9.5764999999999993</v>
+      </c>
+      <c r="O177" s="28"/>
+      <c r="P177" s="4">
+        <f>MAX(D177:F177)</f>
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="Q177" s="4">
+        <f>MIN(D177:F177)</f>
+        <v>9.3629999999999995</v>
+      </c>
+      <c r="R177" s="13">
+        <f>N161/N177</f>
+        <v>67.873711690074671</v>
+      </c>
+    </row>
+    <row r="178" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B178" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C178" s="4">
+        <v>24</v>
+      </c>
+      <c r="D178">
+        <v>8.8759999999999994</v>
+      </c>
+      <c r="E178">
+        <v>7.6890000000000001</v>
+      </c>
+      <c r="N178" s="27">
+        <f t="shared" si="22"/>
+        <v>8.2824999999999989</v>
+      </c>
+      <c r="O178" s="28"/>
+      <c r="P178" s="4">
+        <f t="shared" si="23"/>
+        <v>8.8759999999999994</v>
+      </c>
+      <c r="Q178" s="4">
+        <f t="shared" si="24"/>
+        <v>7.6890000000000001</v>
+      </c>
+      <c r="R178" s="13">
+        <f>N161/N178</f>
+        <v>78.477826743133122</v>
+      </c>
+    </row>
+    <row r="179" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B179" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C179" s="4">
+        <v>25</v>
+      </c>
+      <c r="D179">
+        <v>7.9530000000000003</v>
+      </c>
+      <c r="E179">
+        <v>7.5010000000000003</v>
+      </c>
+      <c r="N179" s="27">
+        <f t="shared" si="22"/>
+        <v>7.7270000000000003</v>
+      </c>
+      <c r="O179" s="28"/>
+      <c r="P179" s="4">
+        <f t="shared" si="23"/>
+        <v>7.9530000000000003</v>
+      </c>
+      <c r="Q179" s="4">
+        <f t="shared" si="24"/>
+        <v>7.5010000000000003</v>
+      </c>
+      <c r="R179" s="13">
+        <f>N161/N179</f>
+        <v>84.119658340882623</v>
+      </c>
+    </row>
+    <row r="180" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B180" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C180" s="5">
+        <v>27</v>
+      </c>
+      <c r="D180" s="15">
+        <v>6.99</v>
+      </c>
+      <c r="E180" s="15">
+        <v>6.8620000000000001</v>
+      </c>
+      <c r="F180" s="15"/>
+      <c r="G180" s="15"/>
+      <c r="H180" s="15"/>
+      <c r="I180" s="15"/>
+      <c r="J180" s="15"/>
+      <c r="K180" s="15"/>
+      <c r="L180" s="15"/>
+      <c r="M180" s="15"/>
+      <c r="N180" s="27">
+        <f t="shared" si="22"/>
+        <v>6.9260000000000002</v>
+      </c>
+      <c r="O180" s="28"/>
+      <c r="P180" s="5">
+        <f t="shared" si="23"/>
+        <v>6.99</v>
+      </c>
+      <c r="Q180" s="5">
+        <f t="shared" si="24"/>
+        <v>6.8620000000000001</v>
+      </c>
+      <c r="R180" s="16">
+        <f>N161/N180</f>
+        <v>93.84819520646839</v>
+      </c>
+    </row>
+    <row r="181" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B181" t="s">
+        <v>65</v>
+      </c>
+      <c r="C181" s="43">
+        <v>32</v>
+      </c>
+      <c r="D181">
+        <v>5.8929999999999998</v>
+      </c>
+      <c r="E181">
+        <v>6.4909999999999997</v>
+      </c>
+      <c r="N181" s="27">
+        <f t="shared" si="22"/>
+        <v>6.1920000000000002</v>
+      </c>
+      <c r="O181" s="28"/>
+      <c r="R181" s="16">
+        <f>N161/N181</f>
+        <v>104.97296511627907</v>
+      </c>
+    </row>
+    <row r="182" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B182" t="s">
+        <v>66</v>
+      </c>
+      <c r="C182" s="43">
+        <v>36</v>
+      </c>
+      <c r="D182">
+        <v>5.4729999999999999</v>
+      </c>
+      <c r="E182">
+        <v>5.4219999999999997</v>
+      </c>
+      <c r="N182" s="27">
+        <f t="shared" si="22"/>
+        <v>5.4474999999999998</v>
+      </c>
+      <c r="O182" s="28"/>
+      <c r="R182" s="16">
+        <f>N161/N182</f>
+        <v>119.31943093162002</v>
+      </c>
+    </row>
+    <row r="183" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B183" t="s">
+        <v>67</v>
+      </c>
+      <c r="C183" s="43">
+        <v>48</v>
+      </c>
+      <c r="D183">
+        <v>4.7830000000000004</v>
+      </c>
+      <c r="E183">
+        <v>4.468</v>
+      </c>
+      <c r="N183" s="27">
+        <f t="shared" si="22"/>
+        <v>4.6255000000000006</v>
+      </c>
+      <c r="O183" s="28"/>
+      <c r="R183" s="16">
+        <f>N161/N183</f>
+        <v>140.52374878391524</v>
+      </c>
+    </row>
+    <row r="184" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B184" t="s">
+        <v>68</v>
+      </c>
+      <c r="C184" s="43">
+        <v>64</v>
+      </c>
+      <c r="D184">
+        <v>4.194</v>
+      </c>
+      <c r="E184">
+        <v>3.8860000000000001</v>
+      </c>
+      <c r="F184">
+        <v>3.9009999999999998</v>
+      </c>
+      <c r="G184">
+        <v>3.4780000000000002</v>
+      </c>
+      <c r="H184">
+        <v>3.5390000000000001</v>
+      </c>
+      <c r="N184" s="27">
+        <f t="shared" si="22"/>
+        <v>3.7996000000000003</v>
+      </c>
+      <c r="O184" s="28"/>
+      <c r="R184" s="16">
+        <f>N161/N184</f>
+        <v>171.06869144120432</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="55">
+    <mergeCell ref="N184:O184"/>
+    <mergeCell ref="N179:O179"/>
+    <mergeCell ref="N180:O180"/>
+    <mergeCell ref="N181:O181"/>
+    <mergeCell ref="N182:O182"/>
+    <mergeCell ref="N183:O183"/>
+    <mergeCell ref="N174:O174"/>
+    <mergeCell ref="N175:O175"/>
+    <mergeCell ref="N176:O176"/>
+    <mergeCell ref="N177:O177"/>
+    <mergeCell ref="N178:O178"/>
+    <mergeCell ref="N169:O169"/>
+    <mergeCell ref="N170:O170"/>
+    <mergeCell ref="N171:O171"/>
+    <mergeCell ref="N172:O172"/>
+    <mergeCell ref="N173:O173"/>
+    <mergeCell ref="N164:O164"/>
+    <mergeCell ref="N165:O165"/>
+    <mergeCell ref="N166:O166"/>
+    <mergeCell ref="N167:O167"/>
+    <mergeCell ref="N168:O168"/>
+    <mergeCell ref="B159:Q159"/>
+    <mergeCell ref="N160:O160"/>
+    <mergeCell ref="N161:O161"/>
+    <mergeCell ref="N162:O162"/>
+    <mergeCell ref="N163:O163"/>
+    <mergeCell ref="B132:R132"/>
+    <mergeCell ref="B131:J131"/>
+    <mergeCell ref="S132:T132"/>
     <mergeCell ref="T83:AI83"/>
     <mergeCell ref="B60:Q60"/>
     <mergeCell ref="AE51:AF51"/>
@@ -13579,7 +16326,7 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>